<commit_message>
ADD: final boxplot + summary table and specific boxplot
</commit_message>
<xml_diff>
--- a/bin/summary_table/RESULT_SUMMARY_FOF.xlsx
+++ b/bin/summary_table/RESULT_SUMMARY_FOF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmatt\Documents\MIALab\bin\summary_table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859AC954-A37F-4EC9-82CF-FDA320370C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7178504E-840B-4F01-8F5A-9D4A22145298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3CEA872F-7358-49E8-9EAA-A7ECE4E8452B}"/>
+    <workbookView minimized="1" xWindow="5895" yWindow="4320" windowWidth="28800" windowHeight="15345" xr2:uid="{3CEA872F-7358-49E8-9EAA-A7ECE4E8452B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,20 +139,12 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Cambria"/>
@@ -168,7 +160,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -296,45 +288,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -365,41 +318,88 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
@@ -410,64 +410,23 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -477,8 +436,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
@@ -490,7 +449,81 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -505,163 +538,133 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -976,1324 +979,1325 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236EB72D-A019-4EC3-8BA8-BEF5E71859F2}">
   <dimension ref="D3:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="24" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="4:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="13" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="15"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="28"/>
     </row>
     <row r="5" spans="4:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="D5" s="11"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="30"/>
+      <c r="G5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="30"/>
+      <c r="I5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
+      <c r="J5" s="30"/>
+      <c r="K5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5" t="s">
+      <c r="L5" s="30"/>
+      <c r="M5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="16" t="s">
+      <c r="N5" s="31"/>
+      <c r="O5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17" t="s">
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17" t="s">
+      <c r="R5" s="33"/>
+      <c r="S5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17" t="s">
+      <c r="T5" s="33"/>
+      <c r="U5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17" t="s">
+      <c r="V5" s="33"/>
+      <c r="W5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="X5" s="18"/>
+      <c r="X5" s="34"/>
     </row>
     <row r="6" spans="4:24" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="12"/>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="O6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P6" s="20" t="s">
+      <c r="P6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="20" t="s">
+      <c r="Q6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="20" t="s">
+      <c r="S6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="T6" s="20" t="s">
+      <c r="T6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="U6" s="20" t="s">
+      <c r="U6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="20" t="s">
+      <c r="V6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W6" s="20" t="s">
+      <c r="W6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="X6" s="21" t="s">
+      <c r="X6" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D7" s="44" t="s">
+    <row r="7" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="39">
+        <v>0.51696048999999999</v>
+      </c>
+      <c r="F7" s="16">
+        <v>3.4682060000000001E-2</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0.50636219000000005</v>
+      </c>
+      <c r="H7" s="16">
+        <v>2.9248349999999999E-2</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0.76055808000000003</v>
+      </c>
+      <c r="J7" s="16">
+        <v>2.794812E-2</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.80650959</v>
+      </c>
+      <c r="L7" s="16">
+        <v>2.0555219999999999E-2</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0.70931613000000004</v>
+      </c>
+      <c r="N7" s="17">
+        <v>8.5145299999999993E-3</v>
+      </c>
+      <c r="O7" s="18">
+        <v>13.230092089999999</v>
+      </c>
+      <c r="P7" s="16">
+        <v>1.40166445</v>
+      </c>
+      <c r="Q7" s="16">
+        <v>13.46717583</v>
+      </c>
+      <c r="R7" s="16">
+        <v>1.0654460100000001</v>
+      </c>
+      <c r="S7" s="16">
+        <v>16.39270084</v>
+      </c>
+      <c r="T7" s="16">
+        <v>1.4419982899999999</v>
+      </c>
+      <c r="U7" s="16">
+        <v>3.86999819</v>
+      </c>
+      <c r="V7" s="16">
+        <v>0.35087611000000002</v>
+      </c>
+      <c r="W7" s="16">
+        <v>2.4873158399999999</v>
+      </c>
+      <c r="X7" s="19">
+        <v>0.64285292999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="40">
         <v>0.52124126999999998</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F8" s="8">
         <v>3.5947489999999999E-2</v>
       </c>
-      <c r="G7" s="47">
+      <c r="G8" s="35">
         <v>0.51517166999999997</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H8" s="8">
         <v>2.917612E-2</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I8" s="8">
         <v>0.75892972999999997</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J8" s="8">
         <v>2.5437620000000001E-2</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K8" s="8">
         <v>0.80551645000000005</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L8" s="8">
         <v>2.0986649999999999E-2</v>
       </c>
-      <c r="M7" s="26">
+      <c r="M8" s="8">
         <v>0.70975219000000001</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N8" s="9">
         <v>8.5491300000000003E-3</v>
       </c>
-      <c r="O7" s="28">
+      <c r="O8" s="37">
         <v>12.370899469999999</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P8" s="8">
         <v>1.3269687999999999</v>
       </c>
-      <c r="Q7" s="26">
+      <c r="Q8" s="35">
         <v>13.102196019999999</v>
       </c>
-      <c r="R7" s="26">
+      <c r="R8" s="8">
         <v>1.01610008</v>
       </c>
-      <c r="S7" s="26">
+      <c r="S8" s="8">
         <v>18.932753349999999</v>
       </c>
-      <c r="T7" s="26">
+      <c r="T8" s="8">
         <v>1.9876746700000001</v>
       </c>
-      <c r="U7" s="26">
+      <c r="U8" s="8">
         <v>3.8788275400000001</v>
       </c>
-      <c r="V7" s="26">
+      <c r="V8" s="8">
         <v>0.39331527999999999</v>
       </c>
-      <c r="W7" s="38">
+      <c r="W8" s="35">
         <v>2.47566255</v>
       </c>
-      <c r="X7" s="39">
+      <c r="X8" s="10">
         <v>0.68636355000000004</v>
       </c>
     </row>
-    <row r="8" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D8" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="41">
+    <row r="9" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="40">
         <v>0.51830125000000005</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F9" s="8">
         <v>3.1933660000000003E-2</v>
       </c>
-      <c r="G8" s="48">
+      <c r="G9" s="35">
         <v>0.52123094000000003</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H9" s="8">
         <v>3.2505239999999998E-2</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I9" s="8">
         <v>0.75949580999999999</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J9" s="8">
         <v>2.8925820000000001E-2</v>
       </c>
-      <c r="K8" s="29">
+      <c r="K9" s="8">
         <v>0.80790101999999997</v>
       </c>
-      <c r="L8" s="29">
+      <c r="L9" s="8">
         <v>2.07729E-2</v>
       </c>
-      <c r="M8" s="29">
+      <c r="M9" s="8">
         <v>0.71012171999999996</v>
       </c>
-      <c r="N8" s="30">
+      <c r="N9" s="9">
         <v>8.4880100000000007E-3</v>
       </c>
-      <c r="O8" s="36">
+      <c r="O9" s="37">
         <v>12.269780340000001</v>
       </c>
-      <c r="P8" s="29">
+      <c r="P9" s="8">
         <v>1.2459897499999999</v>
       </c>
-      <c r="Q8" s="29">
+      <c r="Q9" s="35">
         <v>13.21243303</v>
       </c>
-      <c r="R8" s="29">
+      <c r="R9" s="8">
         <v>0.91192846000000005</v>
       </c>
-      <c r="S8" s="35">
+      <c r="S9" s="8">
         <v>17.64794187</v>
       </c>
-      <c r="T8" s="29">
+      <c r="T9" s="8">
         <v>3.4568986000000002</v>
       </c>
-      <c r="U8" s="35">
+      <c r="U9" s="35">
         <v>3.7523526500000002</v>
       </c>
-      <c r="V8" s="29">
+      <c r="V9" s="8">
         <v>0.34619298999999998</v>
       </c>
-      <c r="W8" s="49">
+      <c r="W9" s="35">
         <v>2.4106715599999999</v>
       </c>
-      <c r="X8" s="23">
+      <c r="X9" s="10">
         <v>0.53727334000000004</v>
       </c>
     </row>
-    <row r="9" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D9" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="41">
-        <v>0.51696048999999999</v>
-      </c>
-      <c r="F9" s="29">
-        <v>3.4682060000000001E-2</v>
-      </c>
-      <c r="G9" s="29">
-        <v>0.50636219000000005</v>
-      </c>
-      <c r="H9" s="29">
-        <v>2.9248349999999999E-2</v>
-      </c>
-      <c r="I9" s="29">
-        <v>0.76055808000000003</v>
-      </c>
-      <c r="J9" s="29">
-        <v>2.794812E-2</v>
-      </c>
-      <c r="K9" s="29">
-        <v>0.80650959</v>
-      </c>
-      <c r="L9" s="29">
-        <v>2.0555219999999999E-2</v>
-      </c>
-      <c r="M9" s="29">
-        <v>0.70931613000000004</v>
-      </c>
-      <c r="N9" s="30">
-        <v>8.5145299999999993E-3</v>
-      </c>
-      <c r="O9" s="31">
-        <v>13.230092089999999</v>
-      </c>
-      <c r="P9" s="29">
-        <v>1.40166445</v>
-      </c>
-      <c r="Q9" s="29">
-        <v>13.46717583</v>
-      </c>
-      <c r="R9" s="29">
-        <v>1.0654460100000001</v>
-      </c>
-      <c r="S9" s="35">
-        <v>16.39270084</v>
-      </c>
-      <c r="T9" s="29">
-        <v>1.4419982899999999</v>
-      </c>
-      <c r="U9" s="29">
-        <v>3.86999819</v>
-      </c>
-      <c r="V9" s="29">
-        <v>0.35087611000000002</v>
-      </c>
-      <c r="W9" s="22">
-        <v>2.4873158399999999</v>
-      </c>
-      <c r="X9" s="23">
-        <v>0.64285292999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D10" s="45" t="s">
+    <row r="10" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="40">
         <v>0.52465914000000002</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="8">
         <v>3.2018280000000003E-2</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="35">
         <v>0.52484176999999999</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="8">
         <v>3.2623680000000002E-2</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="8">
         <v>0.75731601999999998</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="8">
         <v>2.908908E-2</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="8">
         <v>0.80719624000000001</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="8">
         <v>2.166533E-2</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="8">
         <v>0.71047168000000005</v>
       </c>
-      <c r="N10" s="30">
+      <c r="N10" s="9">
         <v>8.8888500000000002E-3</v>
       </c>
-      <c r="O10" s="36">
+      <c r="O10" s="37">
         <v>12.1868249</v>
       </c>
-      <c r="P10" s="29">
+      <c r="P10" s="8">
         <v>1.29664907</v>
       </c>
-      <c r="Q10" s="29">
+      <c r="Q10" s="35">
         <v>13.32796594</v>
       </c>
-      <c r="R10" s="29">
+      <c r="R10" s="8">
         <v>0.87482800000000005</v>
       </c>
-      <c r="S10" s="35">
+      <c r="S10" s="8">
         <v>17.043188910000001</v>
       </c>
-      <c r="T10" s="29">
+      <c r="T10" s="8">
         <v>0.91088524999999998</v>
       </c>
       <c r="U10" s="35">
         <v>3.5961456599999999</v>
       </c>
-      <c r="V10" s="29">
+      <c r="V10" s="8">
         <v>0.40955636000000001</v>
       </c>
-      <c r="W10" s="49">
+      <c r="W10" s="35">
         <v>2.4322648199999999</v>
       </c>
-      <c r="X10" s="23">
+      <c r="X10" s="10">
         <v>0.61974821000000002</v>
       </c>
     </row>
-    <row r="11" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D11" s="45" t="s">
+    <row r="11" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="40">
         <v>0.52048989999999995</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="8">
         <v>3.5667150000000002E-2</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="8">
         <v>0.50698544999999995</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="8">
         <v>2.9503580000000001E-2</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="8">
         <v>0.76177563999999998</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="8">
         <v>2.6792799999999999E-2</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11" s="8">
         <v>0.80632185000000001</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="8">
         <v>2.0614090000000002E-2</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="8">
         <v>0.70935243000000003</v>
       </c>
-      <c r="N11" s="30">
+      <c r="N11" s="9">
         <v>8.5318600000000005E-3</v>
       </c>
-      <c r="O11" s="31">
+      <c r="O11" s="37">
         <v>12.98209452</v>
       </c>
-      <c r="P11" s="29">
+      <c r="P11" s="8">
         <v>1.4018637199999999</v>
       </c>
-      <c r="Q11" s="29">
+      <c r="Q11" s="35">
         <v>13.37140617</v>
       </c>
-      <c r="R11" s="29">
+      <c r="R11" s="8">
         <v>1.00274475</v>
       </c>
       <c r="S11" s="35">
         <v>15.95047411</v>
       </c>
-      <c r="T11" s="29">
+      <c r="T11" s="8">
         <v>1.8391236099999999</v>
       </c>
       <c r="U11" s="35">
         <v>3.8577745399999999</v>
       </c>
-      <c r="V11" s="29">
+      <c r="V11" s="35">
         <v>0.34289303999999998</v>
       </c>
-      <c r="W11" s="49">
+      <c r="W11" s="35">
         <v>2.4701585599999998</v>
       </c>
-      <c r="X11" s="23">
+      <c r="X11" s="10">
         <v>0.63112336999999996</v>
       </c>
     </row>
-    <row r="12" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="45" t="s">
+    <row r="12" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="40">
         <v>0.52159811</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="8">
         <v>3.5250240000000002E-2</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="35">
         <v>0.51993423000000005</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="8">
         <v>2.6790720000000001E-2</v>
       </c>
-      <c r="I12" s="29">
+      <c r="I12" s="8">
         <v>0.76016824999999999</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="8">
         <v>2.70397E-2</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="8">
         <v>0.80711319999999998</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="8">
         <v>2.0436639999999999E-2</v>
       </c>
-      <c r="M12" s="29">
+      <c r="M12" s="8">
         <v>0.70908506999999998</v>
       </c>
-      <c r="N12" s="30">
+      <c r="N12" s="9">
         <v>8.4197200000000003E-3</v>
       </c>
-      <c r="O12" s="31">
+      <c r="O12" s="37">
         <v>12.39977569</v>
       </c>
-      <c r="P12" s="29">
+      <c r="P12" s="8">
         <v>1.24320663</v>
       </c>
-      <c r="Q12" s="29">
+      <c r="Q12" s="8">
         <v>13.4904119</v>
       </c>
-      <c r="R12" s="29">
+      <c r="R12" s="8">
         <v>1.58391499</v>
       </c>
-      <c r="S12" s="35">
+      <c r="S12" s="8">
         <v>16.660988849999999</v>
       </c>
-      <c r="T12" s="29">
+      <c r="T12" s="8">
         <v>0.84347536000000001</v>
       </c>
-      <c r="U12" s="29">
+      <c r="U12" s="8">
         <v>3.93988966</v>
       </c>
-      <c r="V12" s="29">
+      <c r="V12" s="8">
         <v>0.27797379999999999</v>
       </c>
-      <c r="W12" s="22">
+      <c r="W12" s="8">
         <v>2.5494221100000001</v>
       </c>
-      <c r="X12" s="23">
+      <c r="X12" s="10">
         <v>0.63280875999999997</v>
       </c>
     </row>
-    <row r="13" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D13" s="45" t="s">
+    <row r="13" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="40">
         <v>0.52342469999999996</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="8">
         <v>3.7297780000000003E-2</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="8">
         <v>0.50386805999999995</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="8">
         <v>2.863096E-2</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="8">
         <v>0.76202504999999998</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="8">
         <v>2.86024E-2</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="8">
         <v>0.80710844999999998</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="8">
         <v>1.8453290000000001E-2</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="8">
         <v>0.70936606999999996</v>
       </c>
-      <c r="N13" s="30">
+      <c r="N13" s="9">
         <v>8.3271700000000001E-3</v>
       </c>
-      <c r="O13" s="31">
+      <c r="O13" s="37">
         <v>12.836054750000001</v>
       </c>
-      <c r="P13" s="29">
+      <c r="P13" s="8">
         <v>1.3174591200000001</v>
       </c>
-      <c r="Q13" s="29">
+      <c r="Q13" s="8">
         <v>13.553452740000001</v>
       </c>
-      <c r="R13" s="29">
+      <c r="R13" s="8">
         <v>0.95074652000000004</v>
       </c>
-      <c r="S13" s="35">
+      <c r="S13" s="8">
         <v>16.385757179999999</v>
       </c>
-      <c r="T13" s="29">
+      <c r="T13" s="8">
         <v>1.00347477</v>
       </c>
-      <c r="U13" s="29">
+      <c r="U13" s="8">
         <v>3.9586877399999998</v>
       </c>
-      <c r="V13" s="29">
+      <c r="V13" s="8">
         <v>0.35887514999999998</v>
       </c>
-      <c r="W13" s="22">
+      <c r="W13" s="8">
         <v>2.65339086</v>
       </c>
-      <c r="X13" s="23">
+      <c r="X13" s="10">
         <v>0.67787681</v>
       </c>
     </row>
-    <row r="14" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D14" s="45" t="s">
+    <row r="14" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="41">
+      <c r="E14" s="40">
         <v>0.51983522999999998</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="8">
         <v>3.4723759999999999E-2</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="35">
         <v>0.51865475999999999</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" s="8">
         <v>3.1280910000000002E-2</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I14" s="8">
         <v>0.75890281999999998</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="8">
         <v>2.7346329999999999E-2</v>
       </c>
-      <c r="K14" s="29">
+      <c r="K14" s="8">
         <v>0.80849024999999997</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="8">
         <v>2.0109410000000001E-2</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="8">
         <v>0.71032317</v>
       </c>
-      <c r="N14" s="30">
+      <c r="N14" s="9">
         <v>8.3477900000000008E-3</v>
       </c>
-      <c r="O14" s="31">
+      <c r="O14" s="37">
         <v>12.601606950000001</v>
       </c>
-      <c r="P14" s="29">
+      <c r="P14" s="8">
         <v>1.30364963</v>
       </c>
-      <c r="Q14" s="29">
+      <c r="Q14" s="35">
         <v>13.33625741</v>
       </c>
-      <c r="R14" s="29">
+      <c r="R14" s="8">
         <v>1.02187977</v>
       </c>
-      <c r="S14" s="35">
+      <c r="S14" s="8">
         <v>17.688405039999999</v>
       </c>
-      <c r="T14" s="29">
+      <c r="T14" s="8">
         <v>3.10166524</v>
       </c>
       <c r="U14" s="35">
         <v>3.8177083999999999</v>
       </c>
-      <c r="V14" s="29">
+      <c r="V14" s="8">
         <v>0.35369846999999999</v>
       </c>
-      <c r="W14" s="22">
+      <c r="W14" s="8">
         <v>2.53005631</v>
       </c>
-      <c r="X14" s="23">
+      <c r="X14" s="10">
         <v>0.63151807000000004</v>
       </c>
     </row>
-    <row r="15" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D15" s="45" t="s">
+    <row r="15" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="41">
+      <c r="E15" s="40">
         <v>0.52377313999999997</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="8">
         <v>3.3454989999999997E-2</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="35">
         <v>0.52249880999999998</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="8">
         <v>3.2254190000000002E-2</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="8">
         <v>0.75890449999999998</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="8">
         <v>2.8838490000000001E-2</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="8">
         <v>0.80694063999999999</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="8">
         <v>2.193726E-2</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="8">
         <v>0.71005560000000001</v>
       </c>
-      <c r="N15" s="30">
+      <c r="N15" s="9">
         <v>9.0807000000000006E-3</v>
       </c>
-      <c r="O15" s="31">
+      <c r="O15" s="37">
         <v>12.46649255</v>
       </c>
-      <c r="P15" s="29">
+      <c r="P15" s="8">
         <v>1.21924711</v>
       </c>
-      <c r="Q15" s="29">
+      <c r="Q15" s="8">
         <v>14.041069220000001</v>
       </c>
-      <c r="R15" s="29">
+      <c r="R15" s="8">
         <v>0.92107287999999998</v>
       </c>
-      <c r="S15" s="35">
+      <c r="S15" s="8">
         <v>16.843489049999999</v>
       </c>
-      <c r="T15" s="29">
+      <c r="T15" s="8">
         <v>0.99843707999999998</v>
       </c>
       <c r="U15" s="35">
+        <v>3.8441639200000002</v>
+      </c>
+      <c r="V15" s="8">
+        <v>0.34986244</v>
+      </c>
+      <c r="W15" s="35">
+        <v>2.4322648199999999</v>
+      </c>
+      <c r="X15" s="10">
+        <v>0.61974821000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="40">
+        <v>0.51813670999999994</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3.5157229999999998E-2</v>
+      </c>
+      <c r="G16" s="35">
+        <v>0.52234665999999996</v>
+      </c>
+      <c r="H16" s="8">
+        <v>2.9154510000000002E-2</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.75754948</v>
+      </c>
+      <c r="J16" s="8">
+        <v>2.8446720000000002E-2</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0.80764648999999999</v>
+      </c>
+      <c r="L16" s="8">
+        <v>2.0113969999999998E-2</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.70983828999999998</v>
+      </c>
+      <c r="N16" s="9">
+        <v>8.4261800000000001E-3</v>
+      </c>
+      <c r="O16" s="37">
+        <v>12.55531764</v>
+      </c>
+      <c r="P16" s="8">
+        <v>1.28996081</v>
+      </c>
+      <c r="Q16" s="35">
+        <v>13.16845831</v>
+      </c>
+      <c r="R16" s="8">
+        <v>0.83168856000000002</v>
+      </c>
+      <c r="S16" s="8">
+        <v>17.14303164</v>
+      </c>
+      <c r="T16" s="8">
+        <v>0.78515360000000001</v>
+      </c>
+      <c r="U16" s="35">
         <v>3.67739386</v>
       </c>
-      <c r="V15" s="29">
+      <c r="V16" s="8">
         <v>0.42044547999999998</v>
       </c>
-      <c r="W15" s="49">
-        <v>2.4322648199999999</v>
-      </c>
-      <c r="X15" s="23">
-        <v>0.61974821000000002</v>
+      <c r="W16" s="8">
+        <v>2.5494221100000001</v>
+      </c>
+      <c r="X16" s="10">
+        <v>0.63280875999999997</v>
       </c>
     </row>
-    <row r="16" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D16" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="41">
-        <v>0.51813670999999994</v>
-      </c>
-      <c r="F16" s="29">
-        <v>3.5157229999999998E-2</v>
-      </c>
-      <c r="G16" s="29">
-        <v>0.52234665999999996</v>
-      </c>
-      <c r="H16" s="29">
-        <v>2.9154510000000002E-2</v>
-      </c>
-      <c r="I16" s="29">
-        <v>0.75754948</v>
-      </c>
-      <c r="J16" s="29">
-        <v>2.8446720000000002E-2</v>
-      </c>
-      <c r="K16" s="29">
-        <v>0.80764648999999999</v>
-      </c>
-      <c r="L16" s="29">
-        <v>2.0113969999999998E-2</v>
-      </c>
-      <c r="M16" s="29">
-        <v>0.70983828999999998</v>
-      </c>
-      <c r="N16" s="30">
-        <v>8.4261800000000001E-3</v>
-      </c>
-      <c r="O16" s="31">
-        <v>12.55531764</v>
-      </c>
-      <c r="P16" s="29">
-        <v>1.28996081</v>
-      </c>
-      <c r="Q16" s="29">
-        <v>13.16845831</v>
-      </c>
-      <c r="R16" s="29">
-        <v>0.83168856000000002</v>
-      </c>
-      <c r="S16" s="35">
-        <v>17.14303164</v>
-      </c>
-      <c r="T16" s="29">
-        <v>0.78515360000000001</v>
-      </c>
-      <c r="U16" s="35">
-        <v>3.8441639200000002</v>
-      </c>
-      <c r="V16" s="29">
-        <v>0.34986244</v>
-      </c>
-      <c r="W16" s="22">
-        <v>2.5494221100000001</v>
-      </c>
-      <c r="X16" s="23">
-        <v>0.63280875999999997</v>
-      </c>
-    </row>
-    <row r="17" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D17" s="45" t="s">
+    <row r="17" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="41">
         <v>0.52511719999999995</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="8">
         <v>3.5420420000000001E-2</v>
       </c>
       <c r="G17" s="35">
         <v>0.53532248999999998</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="8">
         <v>3.5901379999999997E-2</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I17" s="8">
         <v>0.76052850999999999</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="8">
         <v>3.0568330000000001E-2</v>
       </c>
-      <c r="K17" s="29">
+      <c r="K17" s="8">
         <v>0.80767904000000001</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="8">
         <v>2.362763E-2</v>
       </c>
-      <c r="M17" s="29">
+      <c r="M17" s="8">
         <v>0.71063714</v>
       </c>
-      <c r="N17" s="30">
+      <c r="N17" s="9">
         <v>9.7288099999999992E-3</v>
       </c>
-      <c r="O17" s="31">
+      <c r="O17" s="37">
         <v>12.60312089</v>
       </c>
-      <c r="P17" s="29">
+      <c r="P17" s="8">
         <v>1.2889312900000001</v>
       </c>
-      <c r="Q17" s="29">
+      <c r="Q17" s="8">
         <v>13.569833190000001</v>
       </c>
-      <c r="R17" s="29">
+      <c r="R17" s="8">
         <v>0.92716083999999999</v>
       </c>
-      <c r="S17" s="35">
+      <c r="S17" s="8">
         <v>18.352670679999999</v>
       </c>
-      <c r="T17" s="29">
+      <c r="T17" s="8">
         <v>1.8919510500000001</v>
       </c>
       <c r="U17" s="35">
         <v>3.5278184399999999</v>
       </c>
-      <c r="V17" s="29">
+      <c r="V17" s="8">
         <v>0.39306115000000003</v>
       </c>
-      <c r="W17" s="49">
+      <c r="W17" s="35">
         <v>2.3895804699999998</v>
       </c>
-      <c r="X17" s="23">
+      <c r="X17" s="10">
         <v>0.62442388999999998</v>
       </c>
     </row>
-    <row r="18" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D18" s="45" t="s">
+    <row r="18" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="40">
         <v>0.52297906000000005</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="8">
         <v>3.5290559999999999E-2</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="8">
         <v>0.51110982999999999</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="8">
         <v>2.9217360000000001E-2</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="8">
         <v>0.76111074000000001</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="8">
         <v>2.7462710000000001E-2</v>
       </c>
-      <c r="K18" s="29">
+      <c r="K18" s="8">
         <v>0.80748092000000005</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="8">
         <v>2.0163569999999999E-2</v>
       </c>
-      <c r="M18" s="29">
+      <c r="M18" s="8">
         <v>0.70914862999999995</v>
       </c>
-      <c r="N18" s="30">
+      <c r="N18" s="9">
         <v>8.2059999999999998E-3</v>
       </c>
-      <c r="O18" s="31">
+      <c r="O18" s="37">
         <v>12.5720525</v>
       </c>
-      <c r="P18" s="29">
+      <c r="P18" s="8">
         <v>1.46406832</v>
       </c>
-      <c r="Q18" s="29">
+      <c r="Q18" s="35">
         <v>13.23299409</v>
       </c>
-      <c r="R18" s="29">
+      <c r="R18" s="8">
         <v>1.0898933399999999</v>
       </c>
-      <c r="S18" s="35">
+      <c r="S18" s="8">
         <v>16.962589550000001</v>
       </c>
-      <c r="T18" s="29">
+      <c r="T18" s="8">
         <v>1.0819222900000001</v>
       </c>
-      <c r="U18" s="29">
+      <c r="U18" s="35">
         <v>3.8041080900000002</v>
       </c>
-      <c r="V18" s="29">
+      <c r="V18" s="8">
         <v>0.35883376</v>
       </c>
-      <c r="W18" s="22">
+      <c r="W18" s="8">
         <v>2.5730014400000001</v>
       </c>
-      <c r="X18" s="23">
+      <c r="X18" s="10">
         <v>0.69257749999999996</v>
       </c>
     </row>
-    <row r="19" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D19" s="45" t="s">
+    <row r="19" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="41">
+      <c r="E19" s="40">
         <v>0.51551097000000001</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="8">
         <v>3.4423679999999998E-2</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="35">
         <v>0.51645697999999995</v>
       </c>
-      <c r="H19" s="29">
+      <c r="H19" s="8">
         <v>3.0443769999999998E-2</v>
       </c>
-      <c r="I19" s="29">
+      <c r="I19" s="8">
         <v>0.75499128999999998</v>
       </c>
-      <c r="J19" s="29">
+      <c r="J19" s="8">
         <v>2.4769510000000002E-2</v>
       </c>
-      <c r="K19" s="29">
+      <c r="K19" s="8">
         <v>0.80905956000000001</v>
       </c>
-      <c r="L19" s="29">
+      <c r="L19" s="8">
         <v>1.822638E-2</v>
       </c>
-      <c r="M19" s="29">
+      <c r="M19" s="8">
         <v>0.71054382999999999</v>
       </c>
-      <c r="N19" s="30">
+      <c r="N19" s="9">
         <v>8.2931099999999994E-3</v>
       </c>
-      <c r="O19" s="31">
+      <c r="O19" s="37">
         <v>12.782926489999999</v>
       </c>
-      <c r="P19" s="29">
+      <c r="P19" s="8">
         <v>1.4130783099999999</v>
       </c>
-      <c r="Q19" s="29">
+      <c r="Q19" s="35">
         <v>13.1122824</v>
       </c>
-      <c r="R19" s="29">
+      <c r="R19" s="8">
         <v>0.98389550999999997</v>
       </c>
-      <c r="S19" s="35">
+      <c r="S19" s="8">
         <v>18.25310369</v>
       </c>
-      <c r="T19" s="29">
+      <c r="T19" s="8">
         <v>1.23458728</v>
       </c>
       <c r="U19" s="35">
         <v>3.7497354999999999</v>
       </c>
-      <c r="V19" s="29">
+      <c r="V19" s="8">
         <v>0.37347518000000002</v>
       </c>
-      <c r="W19" s="22">
+      <c r="W19" s="8">
         <v>2.5371115400000002</v>
       </c>
-      <c r="X19" s="23">
+      <c r="X19" s="10">
         <v>0.60254876000000002</v>
       </c>
     </row>
-    <row r="20" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D20" s="45" t="s">
+    <row r="20" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="41">
         <v>0.52738350000000001</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="8">
         <v>3.4223459999999997E-2</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="35">
         <v>0.5237366</v>
       </c>
-      <c r="H20" s="29">
+      <c r="H20" s="8">
         <v>3.2667050000000003E-2</v>
       </c>
-      <c r="I20" s="29">
+      <c r="I20" s="8">
         <v>0.75659299000000002</v>
       </c>
-      <c r="J20" s="29">
+      <c r="J20" s="8">
         <v>2.7851230000000001E-2</v>
       </c>
-      <c r="K20" s="29">
+      <c r="K20" s="8">
         <v>0.80711763999999997</v>
       </c>
-      <c r="L20" s="29">
+      <c r="L20" s="8">
         <v>2.1915190000000001E-2</v>
       </c>
-      <c r="M20" s="29">
+      <c r="M20" s="8">
         <v>0.71047894</v>
       </c>
-      <c r="N20" s="30">
+      <c r="N20" s="9">
         <v>8.9881900000000001E-3</v>
       </c>
-      <c r="O20" s="36">
+      <c r="O20" s="37">
         <v>12.29911077</v>
       </c>
-      <c r="P20" s="29">
+      <c r="P20" s="8">
         <v>1.3160069599999999</v>
       </c>
-      <c r="Q20" s="29">
+      <c r="Q20" s="8">
         <v>13.671207539999999</v>
       </c>
-      <c r="R20" s="29">
+      <c r="R20" s="8">
         <v>0.94767314999999996</v>
       </c>
-      <c r="S20" s="35">
+      <c r="S20" s="8">
         <v>16.887396249999998</v>
       </c>
-      <c r="T20" s="29">
+      <c r="T20" s="8">
         <v>1.05633708</v>
       </c>
-      <c r="U20" s="29">
+      <c r="U20" s="35">
         <v>3.6219799199999998</v>
       </c>
-      <c r="V20" s="29">
+      <c r="V20" s="8">
         <v>0.42574813</v>
       </c>
-      <c r="W20" s="49">
+      <c r="W20" s="35">
         <v>2.39437108</v>
       </c>
-      <c r="X20" s="23">
+      <c r="X20" s="10">
         <v>0.60579461999999995</v>
       </c>
     </row>
-    <row r="21" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D21" s="45" t="s">
+    <row r="21" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="40">
         <v>0.51789816</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="8">
         <v>3.8636940000000002E-2</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="8">
         <v>0.50667905000000002</v>
       </c>
-      <c r="H21" s="29">
+      <c r="H21" s="8">
         <v>3.139517E-2</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="8">
         <v>0.76135631999999998</v>
       </c>
-      <c r="J21" s="29">
+      <c r="J21" s="8">
         <v>2.6590030000000001E-2</v>
       </c>
       <c r="K21" s="35">
         <v>0.82119374999999994</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="8">
         <v>1.177311E-2</v>
       </c>
-      <c r="M21" s="29">
+      <c r="M21" s="8">
         <v>0.71298236000000004</v>
       </c>
-      <c r="N21" s="30">
+      <c r="N21" s="9">
         <v>6.9356699999999997E-3</v>
       </c>
-      <c r="O21" s="31">
+      <c r="O21" s="37">
         <v>12.773715749999999</v>
       </c>
-      <c r="P21" s="29">
+      <c r="P21" s="8">
         <v>1.31612533</v>
       </c>
-      <c r="Q21" s="29">
+      <c r="Q21" s="8">
         <v>14.65606753</v>
       </c>
-      <c r="R21" s="29">
+      <c r="R21" s="8">
         <v>0.63220600000000005</v>
       </c>
-      <c r="S21" s="35">
+      <c r="S21" s="8">
         <v>16.54550214</v>
       </c>
-      <c r="T21" s="29">
+      <c r="T21" s="8">
         <v>0.97280977000000002</v>
       </c>
-      <c r="U21" s="29">
+      <c r="U21" s="35">
         <v>3.8416257100000002</v>
       </c>
-      <c r="V21" s="29">
+      <c r="V21" s="8">
         <v>0.37671197000000001</v>
       </c>
-      <c r="W21" s="22">
+      <c r="W21" s="8">
         <v>2.8023141800000002</v>
       </c>
-      <c r="X21" s="23">
+      <c r="X21" s="10">
         <v>0.80438500999999996</v>
       </c>
     </row>
-    <row r="22" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D22" s="45" t="s">
+    <row r="22" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="41">
+      <c r="E22" s="40">
         <v>0.52465914000000002</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="8">
         <v>3.2018280000000003E-2</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="35">
         <v>0.52484176999999999</v>
       </c>
-      <c r="H22" s="29">
+      <c r="H22" s="8">
         <v>3.2623680000000002E-2</v>
       </c>
-      <c r="I22" s="29">
+      <c r="I22" s="8">
         <v>0.75731601999999998</v>
       </c>
-      <c r="J22" s="29">
+      <c r="J22" s="8">
         <v>2.908908E-2</v>
       </c>
-      <c r="K22" s="29">
+      <c r="K22" s="8">
         <v>0.80719624000000001</v>
       </c>
-      <c r="L22" s="29">
+      <c r="L22" s="8">
         <v>2.166533E-2</v>
       </c>
-      <c r="M22" s="29">
+      <c r="M22" s="8">
         <v>0.71047168000000005</v>
       </c>
-      <c r="N22" s="30">
+      <c r="N22" s="9">
         <v>8.8888500000000002E-3</v>
       </c>
-      <c r="O22" s="36">
+      <c r="O22" s="37">
         <v>12.1868249</v>
       </c>
-      <c r="P22" s="29">
+      <c r="P22" s="8">
         <v>1.29664907</v>
       </c>
-      <c r="Q22" s="29">
+      <c r="Q22" s="35">
         <v>13.32796594</v>
       </c>
-      <c r="R22" s="29">
+      <c r="R22" s="8">
         <v>0.87482800000000005</v>
       </c>
-      <c r="S22" s="35">
+      <c r="S22" s="8">
         <v>17.043188910000001</v>
       </c>
-      <c r="T22" s="29">
+      <c r="T22" s="8">
         <v>0.91088524999999998</v>
       </c>
       <c r="U22" s="35">
         <v>3.5961456599999999</v>
       </c>
-      <c r="V22" s="29">
+      <c r="V22" s="8">
         <v>0.40955636000000001</v>
       </c>
-      <c r="W22" s="49">
+      <c r="W22" s="35">
         <v>2.4322648199999999</v>
       </c>
-      <c r="X22" s="23">
+      <c r="X22" s="10">
         <v>0.61974821000000002</v>
       </c>
     </row>
-    <row r="23" spans="4:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D23" s="45" t="s">
+    <row r="23" spans="4:24" ht="18" x14ac:dyDescent="0.25">
+      <c r="D23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="41">
+      <c r="E23" s="40">
         <v>0.51859701000000002</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="8">
         <v>3.570127E-2</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="8">
         <v>0.50745450000000003</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="8">
         <v>2.9760760000000001E-2</v>
       </c>
-      <c r="I23" s="29">
+      <c r="I23" s="8">
         <v>0.76094289999999998</v>
       </c>
-      <c r="J23" s="29">
+      <c r="J23" s="8">
         <v>2.726818E-2</v>
       </c>
-      <c r="K23" s="29">
+      <c r="K23" s="8">
         <v>0.80655281999999995</v>
       </c>
-      <c r="L23" s="29">
+      <c r="L23" s="8">
         <v>2.0593759999999999E-2</v>
       </c>
-      <c r="M23" s="29">
+      <c r="M23" s="8">
         <v>0.70933900999999999</v>
       </c>
-      <c r="N23" s="30">
+      <c r="N23" s="9">
         <v>8.5276399999999995E-3</v>
       </c>
-      <c r="O23" s="31">
+      <c r="O23" s="37">
         <v>13.02711262</v>
       </c>
-      <c r="P23" s="29">
+      <c r="P23" s="8">
         <v>1.4471823399999999</v>
       </c>
-      <c r="Q23" s="29">
+      <c r="Q23" s="35">
         <v>13.428216770000001</v>
       </c>
-      <c r="R23" s="29">
+      <c r="R23" s="8">
         <v>1.0406701</v>
       </c>
-      <c r="S23" s="35">
+      <c r="S23" s="8">
         <v>16.36478091</v>
       </c>
-      <c r="T23" s="29">
+      <c r="T23" s="8">
         <v>1.8957705300000001</v>
       </c>
-      <c r="U23" s="29">
+      <c r="U23" s="8">
         <v>3.86999819</v>
       </c>
-      <c r="V23" s="29">
+      <c r="V23" s="8">
         <v>0.35087611000000002</v>
       </c>
-      <c r="W23" s="49">
+      <c r="W23" s="35">
         <v>2.4701585599999998</v>
       </c>
-      <c r="X23" s="23">
+      <c r="X23" s="10">
         <v>0.63112336999999996</v>
       </c>
     </row>
-    <row r="24" spans="4:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="46" t="s">
+    <row r="24" spans="4:24" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="42">
         <v>0.52076686999999999</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="12">
         <v>3.5135069999999997E-2</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="36">
         <v>0.52346391999999997</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="12">
         <v>2.8109990000000001E-2</v>
       </c>
-      <c r="I24" s="32">
+      <c r="I24" s="12">
         <v>0.75502822000000003</v>
       </c>
-      <c r="J24" s="32">
+      <c r="J24" s="12">
         <v>2.722989E-2</v>
       </c>
-      <c r="K24" s="32">
+      <c r="K24" s="12">
         <v>0.80776926000000004</v>
       </c>
-      <c r="L24" s="32">
+      <c r="L24" s="12">
         <v>1.953941E-2</v>
       </c>
-      <c r="M24" s="32">
+      <c r="M24" s="12">
         <v>0.71045809999999998</v>
       </c>
-      <c r="N24" s="33">
+      <c r="N24" s="13">
         <v>8.2982200000000002E-3</v>
       </c>
-      <c r="O24" s="34">
+      <c r="O24" s="38">
         <v>12.60294206</v>
       </c>
-      <c r="P24" s="32">
+      <c r="P24" s="12">
         <v>1.25133988</v>
       </c>
-      <c r="Q24" s="32">
+      <c r="Q24" s="36">
         <v>12.855472199999999</v>
       </c>
-      <c r="R24" s="32">
+      <c r="R24" s="12">
         <v>0.96790206999999995</v>
       </c>
-      <c r="S24" s="37">
+      <c r="S24" s="12">
         <v>17.785644829999999</v>
       </c>
-      <c r="T24" s="32">
+      <c r="T24" s="12">
         <v>0.81904694</v>
       </c>
-      <c r="U24" s="32">
+      <c r="U24" s="35">
         <v>3.8195427999999998</v>
       </c>
-      <c r="V24" s="32">
+      <c r="V24" s="12">
         <v>0.33330588</v>
       </c>
-      <c r="W24" s="24">
+      <c r="W24" s="12">
         <v>2.5494221100000001</v>
       </c>
-      <c r="X24" s="25">
+      <c r="X24" s="14">
         <v>0.63280875999999997</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D4:D6"/>
     <mergeCell ref="E4:N4"/>
     <mergeCell ref="O4:X4"/>
     <mergeCell ref="E5:F5"/>
@@ -2306,7 +2310,6 @@
     <mergeCell ref="S5:T5"/>
     <mergeCell ref="U5:V5"/>
     <mergeCell ref="W5:X5"/>
-    <mergeCell ref="D4:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>